<commit_message>
Fix: some completions error && add move to ending shortcut because of "End" Key is far
</commit_message>
<xml_diff>
--- a/Home_WritingCat/repository/Structured Collocations Exeample.xlsx
+++ b/Home_WritingCat/repository/Structured Collocations Exeample.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\writingHelper\Home_WritingCat\repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3076410F-EB3C-4DE9-8418-A986CDC0CFDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BFDC29-4B13-48C8-9158-BB1D86C5CC8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{489BDAD6-CB6B-4906-BCD2-586DEE0C84BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="289">
   <si>
     <t>zero-sum game</t>
   </si>
@@ -1164,6 +1165,10 @@
   </si>
   <si>
     <t>manage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work's closely with</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1562,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C852DF-D2A1-435D-B58E-339D156780E5}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3244,4 +3249,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4859F9C6-9D37-4857-802C-84CC351AC29C}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
todo: should append lackedInterpretations in current Interpretations,waiting mongodb
</commit_message>
<xml_diff>
--- a/Home_WritingCat/repository/Structured Collocations Exeample.xlsx
+++ b/Home_WritingCat/repository/Structured Collocations Exeample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\writingHelper\Home_WritingCat\repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BFDC29-4B13-48C8-9158-BB1D86C5CC8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD71E48-0909-493C-A7B4-EB63503CCC95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{489BDAD6-CB6B-4906-BCD2-586DEE0C84BC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="291">
   <si>
     <t>zero-sum game</t>
   </si>
@@ -1055,18 +1055,9 @@
     <t>生活技能</t>
   </si>
   <si>
-    <t>make a cup of coffee</t>
-  </si>
-  <si>
-    <t>make a cup of tea</t>
-  </si>
-  <si>
     <t>泡一杯茶</t>
   </si>
   <si>
-    <t>make noise</t>
-  </si>
-  <si>
     <t>制造噪音</t>
   </si>
   <si>
@@ -1074,23 +1065,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>make the bed</t>
-  </si>
-  <si>
     <t>整理睡觉的床</t>
   </si>
   <si>
-    <t>make a business deal</t>
-  </si>
-  <si>
     <t>做生意</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>make a fuss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>大惊小怪</t>
   </si>
   <si>
@@ -1100,76 +1081,97 @@
     <t>使…有意义</t>
   </si>
   <si>
+    <t>好理解的</t>
+  </si>
+  <si>
+    <t>合情合理的</t>
+  </si>
+  <si>
+    <t>意味着</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为...安排/腾出时间</t>
+  </si>
+  <si>
+    <t>improve their organization skills</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高他们的组织能力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>it</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>manage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Religion wants make sense of the world.</t>
-  </si>
-  <si>
-    <t>make sense</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>好理解的</t>
-  </si>
-  <si>
-    <t>I feel like a lot of how you structure things make sense to me.</t>
-  </si>
-  <si>
-    <t>合情合理的</t>
-  </si>
-  <si>
-    <t>It seemed to make sense.</t>
-  </si>
-  <si>
-    <t>意味着</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>it make sense that we are special!</t>
-  </si>
-  <si>
-    <t>make time for</t>
-  </si>
-  <si>
-    <t>为...安排/腾出时间</t>
-  </si>
-  <si>
-    <t>manage their time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>improve their organization skills</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高他们的组织能力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>it</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>it is no surprise that</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>it is believed that</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>life skills</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>make</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>manage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>work's closely with</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make sense</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Religion wants make sense of the world.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make sense</t>
+  </si>
+  <si>
+    <t>I feel like a lot of how you structure things make sense to me.</t>
+  </si>
+  <si>
+    <t>It seemed to make sense.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> collocation</t>
+  </si>
+  <si>
+    <t>it is no surprise that</t>
+  </si>
+  <si>
+    <t>it is believed that</t>
+  </si>
+  <si>
+    <t>life skills</t>
+  </si>
+  <si>
+    <t>make a cup of coffee</t>
+  </si>
+  <si>
+    <t>make a cup of tea</t>
+  </si>
+  <si>
+    <t>make noise</t>
+  </si>
+  <si>
+    <t>make the bed</t>
+  </si>
+  <si>
+    <t>make a business deal</t>
+  </si>
+  <si>
+    <t>make a fuss</t>
+  </si>
+  <si>
+    <t>it make sense that we are special!</t>
+  </si>
+  <si>
+    <t>make time for</t>
+  </si>
+  <si>
+    <t>manage their time</t>
   </si>
 </sst>
 </file>
@@ -1567,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C852DF-D2A1-435D-B58E-339D156780E5}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1577,8 +1579,7 @@
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="59.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,7 +1593,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>240</v>
+        <v>278</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>235</v>
@@ -2968,10 +2969,10 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D81" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E81" t="s">
         <v>252</v>
@@ -2985,10 +2986,10 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D82" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E82" t="s">
         <v>253</v>
@@ -3005,7 +3006,7 @@
         <v>247</v>
       </c>
       <c r="D83" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E83" t="s">
         <v>254</v>
@@ -3019,13 +3020,13 @@
         <v>247</v>
       </c>
       <c r="C84" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D84" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="E84" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3036,13 +3037,13 @@
         <v>247</v>
       </c>
       <c r="C85" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D85" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="E85" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3053,13 +3054,13 @@
         <v>247</v>
       </c>
       <c r="C86" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D86" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="E86" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3070,13 +3071,13 @@
         <v>247</v>
       </c>
       <c r="C87" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D87" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="E87" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3087,13 +3088,13 @@
         <v>6</v>
       </c>
       <c r="C88" t="s">
+        <v>270</v>
+      </c>
+      <c r="D88" t="s">
         <v>286</v>
       </c>
-      <c r="D88" t="s">
-        <v>263</v>
-      </c>
       <c r="E88" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3104,13 +3105,13 @@
         <v>247</v>
       </c>
       <c r="C89" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D89" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="E89" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3121,16 +3122,16 @@
         <v>247</v>
       </c>
       <c r="C90" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D90" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="E90" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G90" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3141,16 +3142,16 @@
         <v>247</v>
       </c>
       <c r="C91" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D91" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="E91" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="G91" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3161,16 +3162,16 @@
         <v>247</v>
       </c>
       <c r="C92" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D92" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E92" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="G92" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3181,16 +3182,16 @@
         <v>247</v>
       </c>
       <c r="C93" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D93" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="E93" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="G93" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3201,13 +3202,13 @@
         <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D94" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="E94" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3218,10 +3219,10 @@
         <v>14</v>
       </c>
       <c r="C95" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="D95" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="E95" t="s">
         <v>251</v>
@@ -3238,10 +3239,10 @@
         <v>31</v>
       </c>
       <c r="D96" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="E96" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3256,12 +3257,13 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3294,17 +3296,20 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
+      <c r="B2" t="s">
+        <v>247</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>270</v>
       </c>
       <c r="D2" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>262</v>
+      </c>
+      <c r="G2" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>